<commit_message>
Add correct excel files
</commit_message>
<xml_diff>
--- a/docs/spec/tables/non-primitives.xlsx
+++ b/docs/spec/tables/non-primitives.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\excel_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goats\Documents\bkchxdi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463148FE-377A-4FED-8D1F-31ECAFEE7B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F25D4A-8E73-4087-B1BD-3F629F9CCBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{80D8C4F5-3D34-44DF-B7D6-9FF257957546}"/>
   </bookViews>
@@ -83,17 +83,17 @@
     <t>let rng = 1:5~1;</t>
   </si>
   <si>
-    <t>let tab1 = new TABLE();</t>
-  </si>
-  <si>
-    <t>let A1 = new CELL(5);</t>
-  </si>
-  <si>
     <t>struct example {
     let id = 1, speaker = "john";
     let country = "au";
 };
 const exampleObj = new example(101, "widget", 19.99);</t>
+  </si>
+  <si>
+    <t>let A1 = new cell(5);</t>
+  </si>
+  <si>
+    <t>let tab1 = new table();</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.3">
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>